<commit_message>
✅ Add test data
</commit_message>
<xml_diff>
--- a/tests/testdata/inputfiles/testdata_20200925-3.xlsx
+++ b/tests/testdata/inputfiles/testdata_20200925-3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\GaussianPlume\tests\testdata\inputfiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\gaussianplume\tests\testdata\inputfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83CB9C3-8E94-47FE-8CC5-B0E2EB13706E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C407C223-7297-4530-A492-CB948AF54E31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="4440" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{443E098A-C250-40DD-B657-123E6A67EA17}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{443E098A-C250-40DD-B657-123E6A67EA17}"/>
   </bookViews>
   <sheets>
     <sheet name="static parameters" sheetId="2" r:id="rId1"/>
@@ -89,9 +89,6 @@
     <t>device_name</t>
   </si>
   <si>
-    <t>C:\Python\GaussianPlume\tests\testdata\inputfiles\testdata_20200925-3_data.csv</t>
-  </si>
-  <si>
     <t>filename_measurement_data</t>
   </si>
   <si>
@@ -99,6 +96,9 @@
   </si>
   <si>
     <t>tc_minimum</t>
+  </si>
+  <si>
+    <t>C:\Projects\gaussianplume\tests\testdata\inputfiles\testdata_20200925-3_data.csv</t>
   </si>
 </sst>
 </file>
@@ -476,7 +476,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -504,7 +504,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>11</v>
@@ -512,7 +512,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="2">
         <v>0.05</v>
@@ -520,10 +520,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -539,7 +539,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C9"/>
     </sheetView>
   </sheetViews>

</xml_diff>